<commit_message>
Lite ändringar och jag är klar med en i första sprinten dock ligger jag lite efter med dom andra
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 1.xlsx
+++ b/Sprint Backlog and Burndown - 1.xlsx
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +75,14 @@
     <font>
       <b/>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -101,10 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +411,7 @@
   <dimension ref="B2:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -411,19 +420,19 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
@@ -444,10 +453,10 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -456,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O4" s="2"/>
     </row>
@@ -468,18 +477,20 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>2</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="2:15">
@@ -490,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -549,20 +560,21 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C9" s="3"/>
       <c r="I9">
         <v>18</v>
       </c>
       <c r="J9">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -571,9 +583,10 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="C10" s="3"/>
       <c r="I10">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Nu sitter jag fast så det blev inte så mycket gjort men som tur är låg jag före vilket gör att jag nu inte ligger efter
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 1.xlsx
+++ b/Sprint Backlog and Burndown - 1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Sprint Backlog and Burndown - 1</t>
   </si>
@@ -112,8 +112,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,47 +408,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O10"/>
+  <dimension ref="B2:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:15" ht="31.5">
+    <row r="2" spans="2:16" ht="31.5">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:16">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4">
         <v>2</v>
       </c>
@@ -464,12 +464,15 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="3">
         <v>6</v>
       </c>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="2:15">
+      <c r="O4" s="3"/>
+      <c r="P4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -488,12 +491,15 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="3">
         <v>2</v>
       </c>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="2:15">
+      <c r="O5" s="3"/>
+      <c r="P5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -504,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -512,10 +518,15 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="2:15">
+      <c r="N6" s="3">
+        <v>4</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -534,10 +545,13 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -556,14 +570,17 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="2:15">
-      <c r="B9" s="3" t="s">
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="I9">
         <v>18</v>
       </c>
@@ -571,7 +588,7 @@
         <v>11</v>
       </c>
       <c r="K9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L9">
         <v>2</v>
@@ -579,14 +596,14 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="2:15">
-      <c r="B10" s="3" t="s">
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="I10">
         <v>20</v>
       </c>
@@ -602,8 +619,8 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Nu är jag klar med denna sprint, imorgon ska jag skriva review och planera nästa sprint. Jag behöver nog lägga till extra funktioner.
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 1.xlsx
+++ b/Sprint Backlog and Burndown - 1.xlsx
@@ -109,11 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +412,7 @@
   <dimension ref="B2:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -545,8 +546,10 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="N7" s="4">
+        <v>2</v>
+      </c>
+      <c r="O7" s="4"/>
       <c r="P7" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fixat Burndown men jag fick göra ett fult knep för att fixa den.
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 1.xlsx
+++ b/Sprint Backlog and Burndown - 1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\GitHub\Scrum\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="24720" windowHeight="12090"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Sprint Backlog and Burndown - 1</t>
   </si>
@@ -63,8 +68,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,11 +126,1032 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$B$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Uppskattning</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$C$35:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="6">
+                  <c:v>Dag 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dag 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dag 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dag 4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dag 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$36:$M$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Idealt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$C$35:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="6">
+                  <c:v>Dag 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dag 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dag 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dag 4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Dag 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$C$37:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1201310624"/>
+        <c:axId val="1201318784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1201310624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1201318784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1201318784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1201310624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>509586</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -167,7 +1193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,9 +1225,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,6 +1260,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -408,16 +1436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:P10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:16" ht="31.5">
+    <row r="2" spans="2:16" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +1468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -473,7 +1501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -500,7 +1528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -527,7 +1555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -554,7 +1582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -573,13 +1601,15 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4"/>
       <c r="P8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
@@ -602,7 +1632,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -624,6 +1654,65 @@
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" t="s">
+        <v>5</v>
+      </c>
+      <c r="M35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="I36">
+        <v>18</v>
+      </c>
+      <c r="J36">
+        <v>11</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="I37">
+        <v>20</v>
+      </c>
+      <c r="J37">
+        <v>15</v>
+      </c>
+      <c r="K37">
+        <v>12</v>
+      </c>
+      <c r="L37">
+        <v>6</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -637,28 +1726,29 @@
     <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ändrat lite. Kommit rätt så långt, nästan för långt jag tror att jag kommer behöva lägga till sprintar
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 1.xlsx
+++ b/Sprint Backlog and Burndown - 1.xlsx
@@ -26,9 +26,6 @@
     <t>Sprint Backlog and Burndown - 1</t>
   </si>
   <si>
-    <t>Skapa grundläggande menylayout för medlemsregistret</t>
-  </si>
-  <si>
     <t>Dag 1</t>
   </si>
   <si>
@@ -47,22 +44,25 @@
     <t>Total Arbetstid</t>
   </si>
   <si>
-    <t>Skapa medlemsklass (För-, efternamn, telefon-, medlemsnummer)</t>
-  </si>
-  <si>
-    <t>Registreringsfunktion av nya medlemmar.</t>
-  </si>
-  <si>
-    <t>Visande av medlemslista</t>
-  </si>
-  <si>
-    <t>Detaljerad vy av medlem</t>
-  </si>
-  <si>
     <t>Idealt</t>
   </si>
   <si>
     <t>Uppskattning</t>
+  </si>
+  <si>
+    <t>Skapa en enkel menylayout för medlemsregistret</t>
+  </si>
+  <si>
+    <t>Skapa medlemsklass  med för, efternamn, telefon och medlemsnummer</t>
+  </si>
+  <si>
+    <t>Registreringsfunktion för nya medlemmar.</t>
+  </si>
+  <si>
+    <t>Funktion att visa medlemslista</t>
+  </si>
+  <si>
+    <t>Visa en detaljerad vy av medlem</t>
   </si>
 </sst>
 </file>
@@ -372,11 +372,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1201310624"/>
-        <c:axId val="1201318784"/>
+        <c:axId val="-1212635728"/>
+        <c:axId val="-1212622128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1201310624"/>
+        <c:axId val="-1212635728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +419,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1201318784"/>
+        <c:crossAx val="-1212622128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -427,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1201318784"/>
+        <c:axId val="-1212622128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,7 +478,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1201310624"/>
+        <c:crossAx val="-1212635728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1440,37 +1440,40 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" t="s">
         <v>6</v>
-      </c>
-      <c r="N2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1498,12 +1501,12 @@
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -1525,12 +1528,12 @@
       </c>
       <c r="O5" s="3"/>
       <c r="P5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I6">
         <v>5</v>
@@ -1552,12 +1555,12 @@
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I7">
         <v>3</v>
@@ -1579,12 +1582,12 @@
       </c>
       <c r="O7" s="4"/>
       <c r="P7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I8">
         <v>3</v>
@@ -1606,12 +1609,12 @@
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2"/>
       <c r="I9">
@@ -1634,7 +1637,7 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2"/>
       <c r="I10">
@@ -1657,24 +1660,24 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
         <v>2</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>3</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>4</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>5</v>
-      </c>
-      <c r="M35" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C36" s="2"/>
       <c r="I36">
@@ -1695,7 +1698,7 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C37" s="2"/>
       <c r="I37">

</xml_diff>

<commit_message>
La till båtfunktion också så jag fick lite att göra, nu är det bara en sprint review kvar sen är jag klar.
</commit_message>
<xml_diff>
--- a/Sprint Backlog and Burndown - 1.xlsx
+++ b/Sprint Backlog and Burndown - 1.xlsx
@@ -372,11 +372,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1212635728"/>
-        <c:axId val="-1212622128"/>
+        <c:axId val="1903027984"/>
+        <c:axId val="1903020912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1212635728"/>
+        <c:axId val="1903027984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +419,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1212622128"/>
+        <c:crossAx val="1903020912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -427,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1212622128"/>
+        <c:axId val="1903020912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,7 +478,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1212635728"/>
+        <c:crossAx val="1903027984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1119,8 +1119,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>509586</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -1128,7 +1128,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>590549</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1440,7 +1440,7 @@
   <dimension ref="B2:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>